<commit_message>
sgi and contact details
</commit_message>
<xml_diff>
--- a/BillAppDocs/Elect Bills copy (1).xlsx
+++ b/BillAppDocs/Elect Bills copy (1).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDB26B3-AD7F-4DD0-8EBF-7EBF017DD1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC89F9B-8C49-48E0-BB55-C6640F826EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1725,6 +1725,354 @@
     <xf numFmtId="38" fontId="21" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="9" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="9" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="5" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="24" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="22" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="22" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="21" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="21" fillId="5" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="22" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="22" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="22" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="22" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="22" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="22" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1749,12 +2097,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1791,15 +2133,9 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1812,9 +2148,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1845,344 +2178,137 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="15" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="28" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="22" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="17" fontId="37" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="37" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="37" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="33" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="21" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="21" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="33" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="22" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="37" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="38" fontId="22" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="22" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="23" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="23" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="24" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="22" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="22" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="5" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="23" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="23" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="23" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="23" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="23" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="23" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="22" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="22" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="22" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="22" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="9" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="9" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="5" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="17" fontId="34" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="34" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2199,134 +2325,8 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="34" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="34" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="33" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="37" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="22" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="33" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="28" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="21" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="22" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="17" fontId="37" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="37" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="37" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2739,8 +2739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A21" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A35" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2763,36 +2763,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="85"/>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="89" t="s">
+      <c r="A1" s="201"/>
+      <c r="B1" s="202"/>
+      <c r="C1" s="202"/>
+      <c r="D1" s="202"/>
+      <c r="E1" s="205" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="90"/>
+      <c r="F1" s="205"/>
+      <c r="G1" s="205"/>
+      <c r="H1" s="205"/>
+      <c r="I1" s="205"/>
+      <c r="J1" s="205"/>
+      <c r="K1" s="205"/>
+      <c r="L1" s="205"/>
+      <c r="M1" s="206"/>
     </row>
     <row r="2" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="87"/>
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="92"/>
+      <c r="A2" s="203"/>
+      <c r="B2" s="204"/>
+      <c r="C2" s="204"/>
+      <c r="D2" s="204"/>
+      <c r="E2" s="207"/>
+      <c r="F2" s="207"/>
+      <c r="G2" s="207"/>
+      <c r="H2" s="207"/>
+      <c r="I2" s="207"/>
+      <c r="J2" s="207"/>
+      <c r="K2" s="207"/>
+      <c r="L2" s="207"/>
+      <c r="M2" s="208"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
@@ -2810,21 +2810,21 @@
       <c r="AB2" s="2"/>
     </row>
     <row r="3" spans="1:28" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="87"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="91" t="s">
+      <c r="A3" s="203"/>
+      <c r="B3" s="204"/>
+      <c r="C3" s="204"/>
+      <c r="D3" s="204"/>
+      <c r="E3" s="207" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="92"/>
+      <c r="F3" s="207"/>
+      <c r="G3" s="207"/>
+      <c r="H3" s="207"/>
+      <c r="I3" s="207"/>
+      <c r="J3" s="207"/>
+      <c r="K3" s="207"/>
+      <c r="L3" s="207"/>
+      <c r="M3" s="208"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
@@ -2842,21 +2842,21 @@
       <c r="AB3" s="2"/>
     </row>
     <row r="4" spans="1:28" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="87"/>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="91" t="s">
+      <c r="A4" s="203"/>
+      <c r="B4" s="204"/>
+      <c r="C4" s="204"/>
+      <c r="D4" s="204"/>
+      <c r="E4" s="207" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="91"/>
-      <c r="L4" s="91"/>
-      <c r="M4" s="92"/>
+      <c r="F4" s="207"/>
+      <c r="G4" s="207"/>
+      <c r="H4" s="207"/>
+      <c r="I4" s="207"/>
+      <c r="J4" s="207"/>
+      <c r="K4" s="207"/>
+      <c r="L4" s="207"/>
+      <c r="M4" s="208"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
@@ -2874,31 +2874,31 @@
       <c r="AB4" s="2"/>
     </row>
     <row r="5" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="93" t="s">
+      <c r="A5" s="197" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="94" t="s">
+      <c r="B5" s="197"/>
+      <c r="C5" s="197"/>
+      <c r="D5" s="197"/>
+      <c r="E5" s="185" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="94"/>
+      <c r="F5" s="185"/>
       <c r="G5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="95" t="s">
+      <c r="I5" s="209" t="s">
         <v>78</v>
       </c>
-      <c r="J5" s="96"/>
-      <c r="K5" s="97"/>
-      <c r="L5" s="94" t="s">
+      <c r="J5" s="210"/>
+      <c r="K5" s="211"/>
+      <c r="L5" s="185" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="94"/>
+      <c r="M5" s="185"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
@@ -2916,14 +2916,14 @@
       <c r="AB5" s="2"/>
     </row>
     <row r="6" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="128"/>
-      <c r="B6" s="125"/>
-      <c r="C6" s="125"/>
-      <c r="D6" s="125"/>
-      <c r="E6" s="129" t="s">
+      <c r="A6" s="237"/>
+      <c r="B6" s="184"/>
+      <c r="C6" s="184"/>
+      <c r="D6" s="184"/>
+      <c r="E6" s="194" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="130"/>
+      <c r="F6" s="195"/>
       <c r="G6" s="4"/>
       <c r="H6" s="52" t="s">
         <v>82</v>
@@ -2931,12 +2931,12 @@
       <c r="I6" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="J6" s="131" t="s">
+      <c r="J6" s="196" t="s">
         <v>83</v>
       </c>
-      <c r="K6" s="125"/>
-      <c r="L6" s="131"/>
-      <c r="M6" s="125"/>
+      <c r="K6" s="184"/>
+      <c r="L6" s="196"/>
+      <c r="M6" s="184"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
@@ -2954,31 +2954,31 @@
       <c r="AB6" s="6"/>
     </row>
     <row r="7" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="93" t="s">
+      <c r="A7" s="197" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="93"/>
-      <c r="C7" s="93"/>
-      <c r="D7" s="93"/>
+      <c r="B7" s="197"/>
+      <c r="C7" s="197"/>
+      <c r="D7" s="197"/>
       <c r="E7" s="51" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="94" t="s">
+      <c r="G7" s="185" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="94"/>
+      <c r="H7" s="185"/>
       <c r="I7" s="7" t="s">
         <v>15</v>
       </c>
       <c r="J7" s="8"/>
-      <c r="K7" s="127" t="s">
+      <c r="K7" s="198" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="127"/>
-      <c r="M7" s="127"/>
+      <c r="L7" s="198"/>
+      <c r="M7" s="198"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
       <c r="P7" s="9"/>
@@ -2996,25 +2996,25 @@
       <c r="AB7" s="6"/>
     </row>
     <row r="8" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="125"/>
-      <c r="B8" s="125"/>
-      <c r="C8" s="125"/>
-      <c r="D8" s="125"/>
+      <c r="A8" s="184"/>
+      <c r="B8" s="184"/>
+      <c r="C8" s="184"/>
+      <c r="D8" s="184"/>
       <c r="E8" s="50" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="50"/>
-      <c r="G8" s="126"/>
-      <c r="H8" s="126"/>
-      <c r="I8" s="93" t="s">
+      <c r="G8" s="236"/>
+      <c r="H8" s="236"/>
+      <c r="I8" s="197" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="93"/>
-      <c r="K8" s="125" t="s">
+      <c r="J8" s="197"/>
+      <c r="K8" s="184" t="s">
         <v>19</v>
       </c>
-      <c r="L8" s="125"/>
-      <c r="M8" s="125"/>
+      <c r="L8" s="184"/>
+      <c r="M8" s="184"/>
       <c r="N8" s="5"/>
       <c r="O8"/>
       <c r="P8"/>
@@ -3032,27 +3032,27 @@
       <c r="AB8" s="11"/>
     </row>
     <row r="9" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="197" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="93"/>
-      <c r="C9" s="93"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="119" t="s">
+      <c r="B9" s="197"/>
+      <c r="C9" s="197"/>
+      <c r="D9" s="197"/>
+      <c r="E9" s="197"/>
+      <c r="F9" s="230" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="120"/>
-      <c r="H9" s="121"/>
-      <c r="I9" s="93" t="s">
+      <c r="G9" s="231"/>
+      <c r="H9" s="232"/>
+      <c r="I9" s="197" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="93"/>
-      <c r="K9" s="127" t="s">
+      <c r="J9" s="197"/>
+      <c r="K9" s="198" t="s">
         <v>23</v>
       </c>
-      <c r="L9" s="127"/>
-      <c r="M9" s="127"/>
+      <c r="L9" s="198"/>
+      <c r="M9" s="198"/>
       <c r="N9"/>
       <c r="O9"/>
       <c r="P9"/>
@@ -3070,14 +3070,14 @@
       <c r="AB9" s="11"/>
     </row>
     <row r="10" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="125"/>
-      <c r="B10" s="125"/>
-      <c r="C10" s="125"/>
-      <c r="D10" s="125"/>
-      <c r="E10" s="125"/>
-      <c r="F10" s="122"/>
-      <c r="G10" s="123"/>
-      <c r="H10" s="124"/>
+      <c r="A10" s="184"/>
+      <c r="B10" s="184"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="184"/>
+      <c r="F10" s="233"/>
+      <c r="G10" s="234"/>
+      <c r="H10" s="235"/>
       <c r="I10" s="51" t="s">
         <v>24</v>
       </c>
@@ -3087,10 +3087,10 @@
       <c r="K10" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="L10" s="94" t="s">
+      <c r="L10" s="185" t="s">
         <v>27</v>
       </c>
-      <c r="M10" s="94"/>
+      <c r="M10" s="185"/>
       <c r="O10"/>
       <c r="P10"/>
       <c r="Q10"/>
@@ -3107,21 +3107,21 @@
       <c r="AB10" s="11"/>
     </row>
     <row r="11" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="140" t="s">
+      <c r="A11" s="186" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="141"/>
-      <c r="C11" s="141"/>
-      <c r="D11" s="142"/>
-      <c r="E11" s="142"/>
-      <c r="F11" s="142"/>
-      <c r="G11" s="142"/>
-      <c r="H11" s="143"/>
+      <c r="B11" s="187"/>
+      <c r="C11" s="187"/>
+      <c r="D11" s="188"/>
+      <c r="E11" s="188"/>
+      <c r="F11" s="188"/>
+      <c r="G11" s="188"/>
+      <c r="H11" s="189"/>
       <c r="I11" s="13"/>
       <c r="J11" s="14"/>
       <c r="K11" s="15"/>
-      <c r="L11" s="144"/>
-      <c r="M11" s="145"/>
+      <c r="L11" s="190"/>
+      <c r="M11" s="191"/>
       <c r="N11"/>
       <c r="O11"/>
       <c r="P11"/>
@@ -3139,21 +3139,21 @@
       <c r="AB11" s="11"/>
     </row>
     <row r="12" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="132" t="s">
+      <c r="A12" s="192" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="133"/>
-      <c r="C12" s="133"/>
-      <c r="D12" s="133"/>
-      <c r="E12" s="133"/>
-      <c r="F12" s="133"/>
+      <c r="B12" s="193"/>
+      <c r="C12" s="193"/>
+      <c r="D12" s="193"/>
+      <c r="E12" s="193"/>
+      <c r="F12" s="193"/>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
       <c r="I12" s="17"/>
       <c r="J12" s="18"/>
       <c r="K12" s="19"/>
-      <c r="L12" s="134"/>
-      <c r="M12" s="135"/>
+      <c r="L12" s="160"/>
+      <c r="M12" s="161"/>
       <c r="N12" s="20"/>
       <c r="O12"/>
       <c r="P12"/>
@@ -3171,21 +3171,21 @@
       <c r="AB12"/>
     </row>
     <row r="13" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="132" t="s">
+      <c r="A13" s="192" t="s">
         <v>88</v>
       </c>
-      <c r="B13" s="133"/>
-      <c r="C13" s="133"/>
-      <c r="D13" s="133"/>
-      <c r="E13" s="133"/>
+      <c r="B13" s="193"/>
+      <c r="C13" s="193"/>
+      <c r="D13" s="193"/>
+      <c r="E13" s="193"/>
       <c r="F13" s="46"/>
       <c r="G13"/>
       <c r="H13"/>
       <c r="I13" s="17"/>
       <c r="J13" s="18"/>
       <c r="K13" s="19"/>
-      <c r="L13" s="134"/>
-      <c r="M13" s="135"/>
+      <c r="L13" s="160"/>
+      <c r="M13" s="161"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
@@ -3203,21 +3203,21 @@
       <c r="AB13"/>
     </row>
     <row r="14" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="136" t="s">
+      <c r="A14" s="199" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="137"/>
-      <c r="C14" s="137"/>
-      <c r="D14" s="137"/>
-      <c r="E14" s="137"/>
+      <c r="B14" s="200"/>
+      <c r="C14" s="200"/>
+      <c r="D14" s="200"/>
+      <c r="E14" s="200"/>
       <c r="F14" s="22"/>
       <c r="G14"/>
       <c r="H14"/>
       <c r="I14" s="17"/>
       <c r="J14" s="18"/>
       <c r="K14" s="19"/>
-      <c r="L14" s="134"/>
-      <c r="M14" s="135"/>
+      <c r="L14" s="160"/>
+      <c r="M14" s="161"/>
       <c r="N14"/>
       <c r="O14"/>
       <c r="P14"/>
@@ -3235,21 +3235,21 @@
       <c r="AB14"/>
     </row>
     <row r="15" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="138" t="s">
+      <c r="A15" s="182" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="139"/>
-      <c r="C15" s="139"/>
-      <c r="D15" s="139"/>
-      <c r="E15" s="139"/>
+      <c r="B15" s="183"/>
+      <c r="C15" s="183"/>
+      <c r="D15" s="183"/>
+      <c r="E15" s="183"/>
       <c r="F15" s="23"/>
       <c r="G15" s="23"/>
       <c r="H15" s="23"/>
       <c r="I15" s="17"/>
       <c r="J15" s="18"/>
       <c r="K15" s="19"/>
-      <c r="L15" s="134"/>
-      <c r="M15" s="135"/>
+      <c r="L15" s="160"/>
+      <c r="M15" s="161"/>
       <c r="N15" s="24"/>
       <c r="O15" s="24"/>
       <c r="P15" s="24"/>
@@ -3267,19 +3267,19 @@
       <c r="AB15" s="24"/>
     </row>
     <row r="16" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="138"/>
-      <c r="B16" s="139"/>
-      <c r="C16" s="139"/>
-      <c r="D16" s="139"/>
-      <c r="E16" s="139"/>
-      <c r="F16" s="139"/>
-      <c r="G16" s="139"/>
-      <c r="H16" s="139"/>
+      <c r="A16" s="182"/>
+      <c r="B16" s="183"/>
+      <c r="C16" s="183"/>
+      <c r="D16" s="183"/>
+      <c r="E16" s="183"/>
+      <c r="F16" s="183"/>
+      <c r="G16" s="183"/>
+      <c r="H16" s="183"/>
       <c r="I16" s="17"/>
       <c r="J16" s="18"/>
       <c r="K16" s="19"/>
-      <c r="L16" s="134"/>
-      <c r="M16" s="135"/>
+      <c r="L16" s="160"/>
+      <c r="M16" s="161"/>
       <c r="N16" s="25"/>
       <c r="O16" s="25"/>
       <c r="P16" s="25"/>
@@ -3288,11 +3288,11 @@
       <c r="A17" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="146" t="s">
+      <c r="B17" s="165" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="146"/>
-      <c r="D17" s="146"/>
+      <c r="C17" s="165"/>
+      <c r="D17" s="165"/>
       <c r="E17" s="49" t="s">
         <v>32</v>
       </c>
@@ -3308,346 +3308,346 @@
       <c r="I17" s="17"/>
       <c r="J17" s="18"/>
       <c r="K17" s="19"/>
-      <c r="L17" s="134"/>
-      <c r="M17" s="135"/>
+      <c r="L17" s="160"/>
+      <c r="M17" s="161"/>
       <c r="N17" s="25"/>
       <c r="O17" s="25"/>
       <c r="P17" s="25"/>
     </row>
     <row r="18" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="147" t="s">
+      <c r="A18" s="166" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="110" t="s">
+      <c r="B18" s="222" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="106">
+      <c r="C18" s="220">
         <v>1798</v>
       </c>
-      <c r="D18" s="107"/>
-      <c r="E18" s="150">
+      <c r="D18" s="174"/>
+      <c r="E18" s="162">
         <v>1800</v>
       </c>
-      <c r="F18" s="152">
+      <c r="F18" s="169">
         <v>1</v>
       </c>
-      <c r="G18" s="155">
+      <c r="G18" s="172">
         <f>E18-C18</f>
         <v>2</v>
       </c>
-      <c r="H18" s="107"/>
+      <c r="H18" s="174"/>
       <c r="I18" s="17"/>
       <c r="J18" s="18"/>
       <c r="K18" s="19"/>
-      <c r="L18" s="134"/>
-      <c r="M18" s="135"/>
+      <c r="L18" s="160"/>
+      <c r="M18" s="161"/>
       <c r="N18" s="25"/>
       <c r="O18" s="25"/>
       <c r="P18" s="25"/>
     </row>
     <row r="19" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="148"/>
-      <c r="B19" s="111"/>
-      <c r="C19" s="108"/>
-      <c r="D19" s="109"/>
-      <c r="E19" s="151"/>
-      <c r="F19" s="153"/>
-      <c r="G19" s="156"/>
-      <c r="H19" s="114"/>
+      <c r="A19" s="167"/>
+      <c r="B19" s="223"/>
+      <c r="C19" s="221"/>
+      <c r="D19" s="176"/>
+      <c r="E19" s="164"/>
+      <c r="F19" s="170"/>
+      <c r="G19" s="173"/>
+      <c r="H19" s="175"/>
       <c r="I19" s="17"/>
       <c r="J19" s="18"/>
       <c r="K19" s="19"/>
-      <c r="L19" s="134"/>
-      <c r="M19" s="135"/>
+      <c r="L19" s="160"/>
+      <c r="M19" s="161"/>
       <c r="N19" s="26"/>
       <c r="V19" s="27"/>
     </row>
     <row r="20" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="148"/>
-      <c r="B20" s="116" t="s">
+      <c r="A20" s="167"/>
+      <c r="B20" s="227" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="112">
+      <c r="C20" s="224">
         <v>9325</v>
       </c>
-      <c r="D20" s="107"/>
-      <c r="E20" s="150">
+      <c r="D20" s="174"/>
+      <c r="E20" s="162">
         <v>9332</v>
       </c>
-      <c r="F20" s="153"/>
-      <c r="G20" s="150">
+      <c r="F20" s="170"/>
+      <c r="G20" s="162">
         <f>E20-C20</f>
         <v>7</v>
       </c>
-      <c r="H20" s="114"/>
+      <c r="H20" s="175"/>
       <c r="I20" s="17"/>
       <c r="J20" s="18"/>
       <c r="K20" s="19"/>
-      <c r="L20" s="134"/>
-      <c r="M20" s="135"/>
+      <c r="L20" s="160"/>
+      <c r="M20" s="161"/>
       <c r="N20" s="26"/>
     </row>
     <row r="21" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="148"/>
-      <c r="B21" s="117"/>
-      <c r="C21" s="113"/>
-      <c r="D21" s="114"/>
-      <c r="E21" s="167"/>
-      <c r="F21" s="153"/>
-      <c r="G21" s="167"/>
-      <c r="H21" s="114"/>
+      <c r="A21" s="167"/>
+      <c r="B21" s="228"/>
+      <c r="C21" s="225"/>
+      <c r="D21" s="175"/>
+      <c r="E21" s="163"/>
+      <c r="F21" s="170"/>
+      <c r="G21" s="163"/>
+      <c r="H21" s="175"/>
       <c r="I21" s="17"/>
       <c r="J21" s="18"/>
       <c r="K21" s="19"/>
-      <c r="L21" s="134"/>
-      <c r="M21" s="135"/>
+      <c r="L21" s="160"/>
+      <c r="M21" s="161"/>
       <c r="N21" s="26"/>
     </row>
     <row r="22" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="149"/>
-      <c r="B22" s="118"/>
-      <c r="C22" s="115"/>
-      <c r="D22" s="109"/>
-      <c r="E22" s="151"/>
-      <c r="F22" s="154"/>
-      <c r="G22" s="151"/>
-      <c r="H22" s="109"/>
+      <c r="A22" s="168"/>
+      <c r="B22" s="229"/>
+      <c r="C22" s="226"/>
+      <c r="D22" s="176"/>
+      <c r="E22" s="164"/>
+      <c r="F22" s="171"/>
+      <c r="G22" s="164"/>
+      <c r="H22" s="176"/>
       <c r="I22" s="28"/>
       <c r="J22" s="29"/>
       <c r="K22" s="30"/>
-      <c r="L22" s="134"/>
-      <c r="M22" s="135"/>
+      <c r="L22" s="160"/>
+      <c r="M22" s="161"/>
       <c r="N22" s="26"/>
     </row>
     <row r="23" spans="1:28" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="157" t="s">
+      <c r="A23" s="177" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="158"/>
-      <c r="C23" s="158"/>
-      <c r="D23" s="158"/>
-      <c r="E23" s="158"/>
-      <c r="F23" s="159" t="s">
+      <c r="B23" s="178"/>
+      <c r="C23" s="178"/>
+      <c r="D23" s="178"/>
+      <c r="E23" s="178"/>
+      <c r="F23" s="179" t="s">
         <v>36</v>
       </c>
-      <c r="G23" s="159"/>
-      <c r="H23" s="160"/>
-      <c r="I23" s="161" t="s">
+      <c r="G23" s="179"/>
+      <c r="H23" s="180"/>
+      <c r="I23" s="159" t="s">
         <v>79</v>
       </c>
-      <c r="J23" s="161"/>
-      <c r="K23" s="161"/>
-      <c r="L23" s="162"/>
-      <c r="M23" s="162"/>
+      <c r="J23" s="159"/>
+      <c r="K23" s="159"/>
+      <c r="L23" s="181"/>
+      <c r="M23" s="181"/>
       <c r="N23" s="26"/>
     </row>
     <row r="24" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="163" t="s">
+      <c r="A24" s="157" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="163"/>
-      <c r="C24" s="163"/>
-      <c r="D24" s="163"/>
+      <c r="B24" s="157"/>
+      <c r="C24" s="157"/>
+      <c r="D24" s="157"/>
       <c r="E24" s="47">
         <f>G18+G20</f>
         <v>9</v>
       </c>
-      <c r="F24" s="164" t="s">
+      <c r="F24" s="158" t="s">
         <v>73</v>
       </c>
-      <c r="G24" s="164"/>
+      <c r="G24" s="158"/>
       <c r="H24" s="83"/>
-      <c r="I24" s="161" t="s">
+      <c r="I24" s="159" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="161"/>
-      <c r="K24" s="161"/>
-      <c r="L24" s="165">
+      <c r="J24" s="159"/>
+      <c r="K24" s="159"/>
+      <c r="L24" s="154">
         <f>H37+E31</f>
         <v>1598.0801799999999</v>
       </c>
-      <c r="M24" s="166"/>
+      <c r="M24" s="155"/>
       <c r="N24" s="26"/>
     </row>
     <row r="25" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="170" t="s">
+      <c r="A25" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="170"/>
-      <c r="C25" s="170"/>
-      <c r="D25" s="170"/>
+      <c r="B25" s="121"/>
+      <c r="C25" s="121"/>
+      <c r="D25" s="121"/>
       <c r="E25" s="31">
         <f>G18*E37+G20*E38</f>
         <v>387.76</v>
       </c>
-      <c r="F25" s="168" t="s">
+      <c r="F25" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="G25" s="168"/>
+      <c r="G25" s="112"/>
       <c r="H25" s="83">
         <v>35</v>
       </c>
-      <c r="I25" s="169" t="s">
+      <c r="I25" s="153" t="s">
         <v>40</v>
       </c>
-      <c r="J25" s="169"/>
-      <c r="K25" s="169"/>
-      <c r="L25" s="165">
+      <c r="J25" s="153"/>
+      <c r="K25" s="153"/>
+      <c r="L25" s="154">
         <v>250</v>
       </c>
-      <c r="M25" s="166"/>
+      <c r="M25" s="155"/>
       <c r="N25" s="26"/>
     </row>
     <row r="26" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="98" t="s">
+      <c r="A26" s="212" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="99"/>
-      <c r="C26" s="99"/>
-      <c r="D26" s="100"/>
-      <c r="E26" s="104">
+      <c r="B26" s="213"/>
+      <c r="C26" s="213"/>
+      <c r="D26" s="214"/>
+      <c r="E26" s="218">
         <f>SUM(E25+H35+H24+E28)*18%</f>
         <v>79.029179999999997</v>
       </c>
-      <c r="F26" s="168" t="s">
+      <c r="F26" s="112" t="s">
         <v>42</v>
       </c>
-      <c r="G26" s="168"/>
+      <c r="G26" s="112"/>
       <c r="H26" s="83">
         <v>25</v>
       </c>
-      <c r="I26" s="169" t="s">
+      <c r="I26" s="153" t="s">
         <v>75</v>
       </c>
-      <c r="J26" s="169"/>
-      <c r="K26" s="169"/>
-      <c r="L26" s="165"/>
-      <c r="M26" s="166"/>
+      <c r="J26" s="153"/>
+      <c r="K26" s="153"/>
+      <c r="L26" s="154"/>
+      <c r="M26" s="155"/>
       <c r="N26" s="26"/>
     </row>
     <row r="27" spans="1:28" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="101"/>
-      <c r="B27" s="102"/>
-      <c r="C27" s="102"/>
-      <c r="D27" s="103"/>
-      <c r="E27" s="105"/>
-      <c r="F27" s="168" t="s">
+      <c r="A27" s="215"/>
+      <c r="B27" s="216"/>
+      <c r="C27" s="216"/>
+      <c r="D27" s="217"/>
+      <c r="E27" s="219"/>
+      <c r="F27" s="112" t="s">
         <v>43</v>
       </c>
-      <c r="G27" s="168"/>
+      <c r="G27" s="112"/>
       <c r="H27" s="83"/>
-      <c r="I27" s="169" t="s">
+      <c r="I27" s="153" t="s">
         <v>44</v>
       </c>
-      <c r="J27" s="169"/>
-      <c r="K27" s="169"/>
-      <c r="L27" s="165">
+      <c r="J27" s="153"/>
+      <c r="K27" s="153"/>
+      <c r="L27" s="154">
         <v>0</v>
       </c>
-      <c r="M27" s="166"/>
+      <c r="M27" s="155"/>
       <c r="N27" s="26"/>
     </row>
     <row r="28" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="170" t="s">
+      <c r="A28" s="121" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="170"/>
-      <c r="C28" s="170"/>
-      <c r="D28" s="170"/>
+      <c r="B28" s="121"/>
+      <c r="C28" s="121"/>
+      <c r="D28" s="121"/>
       <c r="E28" s="31">
         <f>E24*2.469</f>
         <v>22.221</v>
       </c>
-      <c r="F28" s="168" t="s">
+      <c r="F28" s="112" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="168"/>
+      <c r="G28" s="112"/>
       <c r="H28" s="83"/>
-      <c r="I28" s="171" t="s">
+      <c r="I28" s="156" t="s">
         <v>49</v>
       </c>
-      <c r="J28" s="171"/>
-      <c r="K28" s="171"/>
-      <c r="L28" s="165">
+      <c r="J28" s="156"/>
+      <c r="K28" s="156"/>
+      <c r="L28" s="154">
         <f>SUM(L24:M25)</f>
         <v>1848.0801799999999</v>
       </c>
-      <c r="M28" s="166"/>
+      <c r="M28" s="155"/>
       <c r="N28" s="26"/>
     </row>
     <row r="29" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="170" t="s">
+      <c r="A29" s="121" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="170"/>
-      <c r="C29" s="170"/>
-      <c r="D29" s="170"/>
+      <c r="B29" s="121"/>
+      <c r="C29" s="121"/>
+      <c r="D29" s="121"/>
       <c r="E29" s="83">
         <v>20</v>
       </c>
-      <c r="F29" s="180" t="s">
+      <c r="F29" s="137" t="s">
         <v>48</v>
       </c>
-      <c r="G29" s="181"/>
-      <c r="H29" s="184"/>
-      <c r="I29" s="186" t="s">
+      <c r="G29" s="138"/>
+      <c r="H29" s="141"/>
+      <c r="I29" s="143" t="s">
         <v>52</v>
       </c>
-      <c r="J29" s="187"/>
-      <c r="K29" s="188"/>
-      <c r="L29" s="192">
+      <c r="J29" s="144"/>
+      <c r="K29" s="145"/>
+      <c r="L29" s="149">
         <f>L31-L28</f>
         <v>184.80801800000017</v>
       </c>
-      <c r="M29" s="193"/>
+      <c r="M29" s="150"/>
       <c r="N29" s="26"/>
     </row>
     <row r="30" spans="1:28" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="170" t="s">
+      <c r="A30" s="121" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="170"/>
-      <c r="C30" s="170"/>
-      <c r="D30" s="170"/>
+      <c r="B30" s="121"/>
+      <c r="C30" s="121"/>
+      <c r="D30" s="121"/>
       <c r="E30" s="83">
         <v>1000</v>
       </c>
-      <c r="F30" s="182"/>
-      <c r="G30" s="183"/>
-      <c r="H30" s="185"/>
-      <c r="I30" s="189"/>
-      <c r="J30" s="190"/>
-      <c r="K30" s="191"/>
-      <c r="L30" s="194"/>
-      <c r="M30" s="195"/>
+      <c r="F30" s="139"/>
+      <c r="G30" s="140"/>
+      <c r="H30" s="142"/>
+      <c r="I30" s="146"/>
+      <c r="J30" s="147"/>
+      <c r="K30" s="148"/>
+      <c r="L30" s="151"/>
+      <c r="M30" s="152"/>
       <c r="N30" s="26"/>
     </row>
     <row r="31" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="172" t="s">
+      <c r="A31" s="129" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="172"/>
-      <c r="C31" s="172"/>
-      <c r="D31" s="172"/>
+      <c r="B31" s="129"/>
+      <c r="C31" s="129"/>
+      <c r="D31" s="129"/>
       <c r="E31" s="31">
         <f>E25+E26+E28+E29+E30</f>
         <v>1509.01018</v>
       </c>
-      <c r="F31" s="168" t="s">
+      <c r="F31" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="G31" s="168"/>
+      <c r="G31" s="112"/>
       <c r="H31" s="83"/>
-      <c r="I31" s="173" t="s">
+      <c r="I31" s="130" t="s">
         <v>55</v>
       </c>
-      <c r="J31" s="173"/>
-      <c r="K31" s="173"/>
-      <c r="L31" s="174">
+      <c r="J31" s="130"/>
+      <c r="K31" s="130"/>
+      <c r="L31" s="131">
         <f>L28*1.1</f>
         <v>2032.8881980000001</v>
       </c>
-      <c r="M31" s="175"/>
+      <c r="M31" s="132"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
@@ -3665,25 +3665,25 @@
       <c r="AB31" s="5"/>
     </row>
     <row r="32" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="170" t="s">
+      <c r="A32" s="121" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="170"/>
-      <c r="C32" s="170"/>
-      <c r="D32" s="170"/>
+      <c r="B32" s="121"/>
+      <c r="C32" s="121"/>
+      <c r="D32" s="121"/>
       <c r="E32" s="31"/>
-      <c r="F32" s="176" t="s">
+      <c r="F32" s="133" t="s">
         <v>54</v>
       </c>
-      <c r="G32" s="176"/>
+      <c r="G32" s="133"/>
       <c r="H32" s="84"/>
-      <c r="I32" s="177" t="s">
+      <c r="I32" s="134" t="s">
         <v>45</v>
       </c>
-      <c r="J32" s="178"/>
-      <c r="K32" s="178"/>
-      <c r="L32" s="178"/>
-      <c r="M32" s="179"/>
+      <c r="J32" s="135"/>
+      <c r="K32" s="135"/>
+      <c r="L32" s="135"/>
+      <c r="M32" s="136"/>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
       <c r="P32" s="5"/>
@@ -3701,29 +3701,29 @@
       <c r="AB32" s="10"/>
     </row>
     <row r="33" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="170" t="s">
+      <c r="A33" s="121" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="170"/>
-      <c r="C33" s="170"/>
-      <c r="D33" s="170"/>
+      <c r="B33" s="121"/>
+      <c r="C33" s="121"/>
+      <c r="D33" s="121"/>
       <c r="E33" s="31"/>
-      <c r="F33" s="168" t="s">
+      <c r="F33" s="112" t="s">
         <v>57</v>
       </c>
-      <c r="G33" s="168"/>
+      <c r="G33" s="112"/>
       <c r="H33" s="83"/>
-      <c r="I33" s="205" t="s">
+      <c r="I33" s="99" t="s">
         <v>60</v>
       </c>
-      <c r="J33" s="207" t="s">
+      <c r="J33" s="123" t="s">
         <v>103</v>
       </c>
-      <c r="K33" s="208"/>
-      <c r="L33" s="209" t="s">
+      <c r="K33" s="124"/>
+      <c r="L33" s="125" t="s">
         <v>64</v>
       </c>
-      <c r="M33" s="210"/>
+      <c r="M33" s="126"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
@@ -3741,27 +3741,27 @@
       <c r="AB33" s="10"/>
     </row>
     <row r="34" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="170" t="s">
+      <c r="A34" s="121" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="170"/>
-      <c r="C34" s="170"/>
-      <c r="D34" s="170"/>
+      <c r="B34" s="121"/>
+      <c r="C34" s="121"/>
+      <c r="D34" s="121"/>
       <c r="E34" s="31"/>
-      <c r="F34" s="168" t="s">
+      <c r="F34" s="112" t="s">
         <v>59</v>
       </c>
-      <c r="G34" s="168"/>
+      <c r="G34" s="112"/>
       <c r="H34" s="83"/>
-      <c r="I34" s="206"/>
-      <c r="J34" s="207" t="s">
+      <c r="I34" s="122"/>
+      <c r="J34" s="123" t="s">
         <v>112</v>
       </c>
-      <c r="K34" s="208"/>
-      <c r="L34" s="211">
+      <c r="K34" s="124"/>
+      <c r="L34" s="127">
         <v>3.5627</v>
       </c>
-      <c r="M34" s="212"/>
+      <c r="M34" s="128"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
@@ -3779,28 +3779,28 @@
       <c r="AB34" s="10"/>
     </row>
     <row r="35" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="196" t="s">
+      <c r="A35" s="111" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="196"/>
-      <c r="C35" s="196"/>
-      <c r="D35" s="196"/>
+      <c r="B35" s="111"/>
+      <c r="C35" s="111"/>
+      <c r="D35" s="111"/>
       <c r="E35" s="31"/>
-      <c r="F35" s="168" t="s">
+      <c r="F35" s="112" t="s">
         <v>63</v>
       </c>
-      <c r="G35" s="168"/>
+      <c r="G35" s="112"/>
       <c r="H35" s="31">
         <f>E24*3.23</f>
         <v>29.07</v>
       </c>
-      <c r="I35" s="197" t="s">
+      <c r="I35" s="113" t="s">
         <v>66</v>
       </c>
-      <c r="J35" s="198"/>
-      <c r="K35" s="198"/>
-      <c r="L35" s="198"/>
-      <c r="M35" s="199"/>
+      <c r="J35" s="114"/>
+      <c r="K35" s="114"/>
+      <c r="L35" s="114"/>
+      <c r="M35" s="115"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
@@ -3821,26 +3821,26 @@
       <c r="A36" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="200" t="s">
+      <c r="B36" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="200"/>
-      <c r="D36" s="200"/>
+      <c r="C36" s="116"/>
+      <c r="D36" s="116"/>
       <c r="E36" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="F36" s="201" t="s">
+      <c r="F36" s="117" t="s">
         <v>65</v>
       </c>
-      <c r="G36" s="201"/>
+      <c r="G36" s="117"/>
       <c r="H36" s="31"/>
-      <c r="I36" s="202" t="s">
+      <c r="I36" s="118" t="s">
         <v>68</v>
       </c>
-      <c r="J36" s="203"/>
-      <c r="K36" s="203"/>
-      <c r="L36" s="203"/>
-      <c r="M36" s="204"/>
+      <c r="J36" s="119"/>
+      <c r="K36" s="119"/>
+      <c r="L36" s="119"/>
+      <c r="M36" s="120"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
@@ -3858,32 +3858,32 @@
       <c r="AB36" s="10"/>
     </row>
     <row r="37" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="205" t="s">
+      <c r="A37" s="99" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="215" t="s">
+      <c r="B37" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="215"/>
-      <c r="D37" s="215"/>
+      <c r="C37" s="87"/>
+      <c r="D37" s="87"/>
       <c r="E37" s="33">
         <v>48</v>
       </c>
-      <c r="F37" s="228" t="s">
+      <c r="F37" s="101" t="s">
         <v>47</v>
       </c>
-      <c r="G37" s="229"/>
+      <c r="G37" s="102"/>
       <c r="H37" s="41">
         <f>SUM(H24:H36)</f>
         <v>89.07</v>
       </c>
-      <c r="I37" s="230" t="s">
+      <c r="I37" s="103" t="s">
         <v>70</v>
       </c>
-      <c r="J37" s="231"/>
-      <c r="K37" s="231"/>
-      <c r="L37" s="231"/>
-      <c r="M37" s="232"/>
+      <c r="J37" s="104"/>
+      <c r="K37" s="104"/>
+      <c r="L37" s="104"/>
+      <c r="M37" s="105"/>
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
@@ -3901,27 +3901,27 @@
       <c r="AB37" s="10"/>
     </row>
     <row r="38" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="227"/>
-      <c r="B38" s="219" t="s">
+      <c r="A38" s="100"/>
+      <c r="B38" s="91" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="219"/>
-      <c r="D38" s="219"/>
+      <c r="C38" s="91"/>
+      <c r="D38" s="91"/>
       <c r="E38" s="34">
         <v>41.68</v>
       </c>
-      <c r="F38" s="233" t="s">
+      <c r="F38" s="106" t="s">
         <v>77</v>
       </c>
-      <c r="G38" s="234"/>
-      <c r="H38" s="235"/>
-      <c r="I38" s="236" t="s">
+      <c r="G38" s="107"/>
+      <c r="H38" s="108"/>
+      <c r="I38" s="109" t="s">
         <v>72</v>
       </c>
-      <c r="J38" s="236"/>
-      <c r="K38" s="236"/>
-      <c r="L38" s="236"/>
-      <c r="M38" s="237"/>
+      <c r="J38" s="109"/>
+      <c r="K38" s="109"/>
+      <c r="L38" s="109"/>
+      <c r="M38" s="110"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
@@ -3939,18 +3939,18 @@
       <c r="AB38" s="10"/>
     </row>
     <row r="39" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="214" t="s">
+      <c r="A39" s="86" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="215"/>
-      <c r="C39" s="215"/>
-      <c r="D39" s="215"/>
+      <c r="B39" s="87"/>
+      <c r="C39" s="87"/>
+      <c r="D39" s="87"/>
       <c r="E39" s="44"/>
-      <c r="F39" s="216" t="s">
+      <c r="F39" s="88" t="s">
         <v>71</v>
       </c>
-      <c r="G39" s="217"/>
-      <c r="H39" s="218"/>
+      <c r="G39" s="89"/>
+      <c r="H39" s="90"/>
       <c r="I39" s="42"/>
       <c r="J39" s="42"/>
       <c r="K39" s="42"/>
@@ -3973,21 +3973,21 @@
       <c r="AB39" s="36"/>
     </row>
     <row r="40" spans="1:28" ht="17.850000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="214"/>
-      <c r="B40" s="219"/>
-      <c r="C40" s="219"/>
-      <c r="D40" s="219"/>
+      <c r="A40" s="86"/>
+      <c r="B40" s="91"/>
+      <c r="C40" s="91"/>
+      <c r="D40" s="91"/>
       <c r="E40" s="45"/>
-      <c r="F40" s="220" t="s">
+      <c r="F40" s="92" t="s">
         <v>89</v>
       </c>
-      <c r="G40" s="221"/>
-      <c r="H40" s="221"/>
-      <c r="I40" s="221"/>
-      <c r="J40" s="221"/>
-      <c r="K40" s="221"/>
-      <c r="L40" s="221"/>
-      <c r="M40" s="222"/>
+      <c r="G40" s="93"/>
+      <c r="H40" s="93"/>
+      <c r="I40" s="93"/>
+      <c r="J40" s="93"/>
+      <c r="K40" s="93"/>
+      <c r="L40" s="93"/>
+      <c r="M40" s="94"/>
       <c r="N40" s="37"/>
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>
@@ -4006,18 +4006,18 @@
     </row>
     <row r="41" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="48"/>
-      <c r="B41" s="226"/>
-      <c r="C41" s="226"/>
-      <c r="D41" s="226"/>
+      <c r="B41" s="98"/>
+      <c r="C41" s="98"/>
+      <c r="D41" s="98"/>
       <c r="E41" s="38"/>
-      <c r="F41" s="223"/>
-      <c r="G41" s="224"/>
-      <c r="H41" s="224"/>
-      <c r="I41" s="224"/>
-      <c r="J41" s="224"/>
-      <c r="K41" s="224"/>
-      <c r="L41" s="224"/>
-      <c r="M41" s="225"/>
+      <c r="F41" s="95"/>
+      <c r="G41" s="96"/>
+      <c r="H41" s="96"/>
+      <c r="I41" s="96"/>
+      <c r="J41" s="96"/>
+      <c r="K41" s="96"/>
+      <c r="L41" s="96"/>
+      <c r="M41" s="97"/>
       <c r="N41" s="6"/>
       <c r="O41" s="6"/>
       <c r="P41" s="5"/>
@@ -4086,10 +4086,10 @@
     <row r="45" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D45" s="40"/>
       <c r="E45" s="6"/>
-      <c r="L45" s="213" t="s">
+      <c r="L45" s="85" t="s">
         <v>76</v>
       </c>
-      <c r="M45" s="213"/>
+      <c r="M45" s="85"/>
       <c r="N45" s="6"/>
       <c r="O45" s="6"/>
       <c r="P45" s="6"/>
@@ -4131,104 +4131,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="122">
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="F40:M41"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="I37:M37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="I38:M38"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="I35:M35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="I36:M36"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="I32:M32"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="F29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="I29:K30"/>
-    <mergeCell ref="L29:M30"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F22"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H22"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="L14:M14"/>
     <mergeCell ref="A1:D4"/>
     <mergeCell ref="E1:M2"/>
     <mergeCell ref="E3:M3"/>
@@ -4253,6 +4155,104 @@
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="K9:M9"/>
     <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F22"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H22"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="I32:M32"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="F29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="I29:K30"/>
+    <mergeCell ref="L29:M30"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="I35:M35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="I36:M36"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="F40:M41"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="I37:M37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="I38:M38"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.35433070866141736" footer="0.31496062992125984"/>
@@ -4287,32 +4287,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="244"/>
-      <c r="B1" s="244"/>
-      <c r="C1" s="282" t="s">
+      <c r="A1" s="246"/>
+      <c r="B1" s="246"/>
+      <c r="C1" s="247" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="282"/>
-      <c r="E1" s="282"/>
-      <c r="F1" s="282"/>
-      <c r="G1" s="282"/>
-      <c r="H1" s="282"/>
-      <c r="I1" s="282"/>
-      <c r="J1" s="282"/>
-      <c r="K1" s="282"/>
+      <c r="D1" s="247"/>
+      <c r="E1" s="247"/>
+      <c r="F1" s="247"/>
+      <c r="G1" s="247"/>
+      <c r="H1" s="247"/>
+      <c r="I1" s="247"/>
+      <c r="J1" s="247"/>
+      <c r="K1" s="247"/>
     </row>
     <row r="2" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="244"/>
-      <c r="B2" s="244"/>
-      <c r="C2" s="282"/>
-      <c r="D2" s="282"/>
-      <c r="E2" s="282"/>
-      <c r="F2" s="282"/>
-      <c r="G2" s="282"/>
-      <c r="H2" s="282"/>
-      <c r="I2" s="282"/>
-      <c r="J2" s="282"/>
-      <c r="K2" s="282"/>
+      <c r="A2" s="246"/>
+      <c r="B2" s="246"/>
+      <c r="C2" s="247"/>
+      <c r="D2" s="247"/>
+      <c r="E2" s="247"/>
+      <c r="F2" s="247"/>
+      <c r="G2" s="247"/>
+      <c r="H2" s="247"/>
+      <c r="I2" s="247"/>
+      <c r="J2" s="247"/>
+      <c r="K2" s="247"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -4323,19 +4323,19 @@
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="244"/>
-      <c r="B3" s="244"/>
-      <c r="C3" s="282" t="s">
+      <c r="A3" s="246"/>
+      <c r="B3" s="246"/>
+      <c r="C3" s="247" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="282"/>
-      <c r="E3" s="282"/>
-      <c r="F3" s="282"/>
-      <c r="G3" s="282"/>
-      <c r="H3" s="282"/>
-      <c r="I3" s="282"/>
-      <c r="J3" s="282"/>
-      <c r="K3" s="282"/>
+      <c r="D3" s="247"/>
+      <c r="E3" s="247"/>
+      <c r="F3" s="247"/>
+      <c r="G3" s="247"/>
+      <c r="H3" s="247"/>
+      <c r="I3" s="247"/>
+      <c r="J3" s="247"/>
+      <c r="K3" s="247"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -4346,19 +4346,19 @@
       <c r="S3" s="2"/>
     </row>
     <row r="4" spans="1:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="244"/>
-      <c r="B4" s="244"/>
-      <c r="C4" s="282" t="s">
+      <c r="A4" s="246"/>
+      <c r="B4" s="246"/>
+      <c r="C4" s="247" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="282"/>
-      <c r="E4" s="282"/>
-      <c r="F4" s="282"/>
-      <c r="G4" s="282"/>
-      <c r="H4" s="282"/>
-      <c r="I4" s="282"/>
-      <c r="J4" s="282"/>
-      <c r="K4" s="282"/>
+      <c r="D4" s="247"/>
+      <c r="E4" s="247"/>
+      <c r="F4" s="247"/>
+      <c r="G4" s="247"/>
+      <c r="H4" s="247"/>
+      <c r="I4" s="247"/>
+      <c r="J4" s="247"/>
+      <c r="K4" s="247"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -4369,29 +4369,29 @@
       <c r="S4" s="2"/>
     </row>
     <row r="5" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="246" t="s">
+      <c r="A5" s="243" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="246"/>
-      <c r="C5" s="278" t="s">
+      <c r="B5" s="243"/>
+      <c r="C5" s="244" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="278"/>
+      <c r="D5" s="244"/>
       <c r="E5" s="54" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="283" t="s">
+      <c r="G5" s="248" t="s">
         <v>90</v>
       </c>
-      <c r="H5" s="284"/>
-      <c r="I5" s="285"/>
-      <c r="J5" s="278" t="s">
+      <c r="H5" s="249"/>
+      <c r="I5" s="250"/>
+      <c r="J5" s="244" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="278"/>
+      <c r="K5" s="244"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -4402,10 +4402,10 @@
       <c r="S5" s="2"/>
     </row>
     <row r="6" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="277"/>
-      <c r="B6" s="277"/>
-      <c r="C6" s="257"/>
-      <c r="D6" s="257"/>
+      <c r="A6" s="238"/>
+      <c r="B6" s="238"/>
+      <c r="C6" s="239"/>
+      <c r="D6" s="239"/>
       <c r="E6" s="56">
         <v>1.5</v>
       </c>
@@ -4415,14 +4415,14 @@
       <c r="G6" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="280" t="s">
+      <c r="H6" s="240" t="s">
         <v>83</v>
       </c>
-      <c r="I6" s="281"/>
-      <c r="J6" s="249" t="s">
+      <c r="I6" s="241"/>
+      <c r="J6" s="242" t="s">
         <v>92</v>
       </c>
-      <c r="K6" s="257"/>
+      <c r="K6" s="239"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
@@ -4433,29 +4433,29 @@
       <c r="S6" s="6"/>
     </row>
     <row r="7" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="246" t="s">
+      <c r="A7" s="243" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="246"/>
+      <c r="B7" s="243"/>
       <c r="C7" s="55" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="278" t="s">
+      <c r="E7" s="244" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="278"/>
-      <c r="G7" s="246" t="s">
+      <c r="F7" s="244"/>
+      <c r="G7" s="243" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="246"/>
-      <c r="I7" s="276" t="s">
+      <c r="H7" s="243"/>
+      <c r="I7" s="245" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="276"/>
-      <c r="K7" s="276"/>
+      <c r="J7" s="245"/>
+      <c r="K7" s="245"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
@@ -4466,25 +4466,25 @@
       <c r="S7" s="6"/>
     </row>
     <row r="8" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="257"/>
-      <c r="B8" s="257"/>
+      <c r="A8" s="239"/>
+      <c r="B8" s="239"/>
       <c r="C8" s="60" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="60">
         <v>3</v>
       </c>
-      <c r="E8" s="277"/>
-      <c r="F8" s="277"/>
-      <c r="G8" s="246" t="s">
+      <c r="E8" s="238"/>
+      <c r="F8" s="238"/>
+      <c r="G8" s="243" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="246"/>
-      <c r="I8" s="257" t="s">
+      <c r="H8" s="243"/>
+      <c r="I8" s="239" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="257"/>
-      <c r="K8" s="257"/>
+      <c r="J8" s="239"/>
+      <c r="K8" s="239"/>
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
@@ -4495,25 +4495,25 @@
       <c r="S8" s="11"/>
     </row>
     <row r="9" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="246" t="s">
+      <c r="A9" s="243" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="246"/>
-      <c r="C9" s="246"/>
-      <c r="D9" s="278" t="s">
+      <c r="B9" s="243"/>
+      <c r="C9" s="243"/>
+      <c r="D9" s="244" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="278"/>
-      <c r="F9" s="278"/>
-      <c r="G9" s="246" t="s">
+      <c r="E9" s="244"/>
+      <c r="F9" s="244"/>
+      <c r="G9" s="243" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="246"/>
-      <c r="I9" s="276">
+      <c r="H9" s="243"/>
+      <c r="I9" s="245">
         <v>0</v>
       </c>
-      <c r="J9" s="276"/>
-      <c r="K9" s="276"/>
+      <c r="J9" s="245"/>
+      <c r="K9" s="245"/>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
@@ -4524,12 +4524,12 @@
       <c r="S9" s="11"/>
     </row>
     <row r="10" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="257"/>
-      <c r="B10" s="257"/>
-      <c r="C10" s="257"/>
+      <c r="A10" s="239"/>
+      <c r="B10" s="239"/>
+      <c r="C10" s="239"/>
       <c r="D10" s="61"/>
-      <c r="E10" s="277"/>
-      <c r="F10" s="277"/>
+      <c r="E10" s="238"/>
+      <c r="F10" s="238"/>
       <c r="G10" s="55" t="s">
         <v>24</v>
       </c>
@@ -4539,10 +4539,10 @@
       <c r="I10" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="278" t="s">
+      <c r="J10" s="244" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="278"/>
+      <c r="K10" s="244"/>
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
@@ -4553,14 +4553,14 @@
       <c r="S10" s="11"/>
     </row>
     <row r="11" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="279" t="s">
+      <c r="A11" s="251" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="279"/>
-      <c r="C11" s="279"/>
-      <c r="D11" s="279"/>
-      <c r="E11" s="279"/>
-      <c r="F11" s="279"/>
+      <c r="B11" s="251"/>
+      <c r="C11" s="251"/>
+      <c r="D11" s="251"/>
+      <c r="E11" s="251"/>
+      <c r="F11" s="251"/>
       <c r="G11" s="62"/>
       <c r="H11" s="63"/>
       <c r="I11" s="64"/>
@@ -4576,14 +4576,14 @@
       <c r="S11" s="11"/>
     </row>
     <row r="12" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="132" t="s">
+      <c r="A12" s="192" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="133"/>
-      <c r="C12" s="133"/>
-      <c r="D12" s="133"/>
-      <c r="E12" s="133"/>
-      <c r="F12" s="133"/>
+      <c r="B12" s="193"/>
+      <c r="C12" s="193"/>
+      <c r="D12" s="193"/>
+      <c r="E12" s="193"/>
+      <c r="F12" s="193"/>
       <c r="G12" s="62"/>
       <c r="H12" s="63"/>
       <c r="I12" s="64"/>
@@ -4599,13 +4599,13 @@
       <c r="S12"/>
     </row>
     <row r="13" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="132" t="s">
+      <c r="A13" s="192" t="s">
         <v>88</v>
       </c>
-      <c r="B13" s="133"/>
-      <c r="C13" s="133"/>
-      <c r="D13" s="133"/>
-      <c r="E13" s="133"/>
+      <c r="B13" s="193"/>
+      <c r="C13" s="193"/>
+      <c r="D13" s="193"/>
+      <c r="E13" s="193"/>
       <c r="F13" s="46"/>
       <c r="G13" s="62"/>
       <c r="H13" s="63"/>
@@ -4628,12 +4628,12 @@
       <c r="Y13"/>
     </row>
     <row r="14" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="270" t="s">
+      <c r="A14" s="259" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="270"/>
-      <c r="C14" s="270"/>
-      <c r="D14" s="270"/>
+      <c r="B14" s="259"/>
+      <c r="C14" s="259"/>
+      <c r="D14" s="259"/>
       <c r="E14" s="66"/>
       <c r="F14" s="66"/>
       <c r="G14" s="62"/>
@@ -4657,12 +4657,12 @@
       <c r="Y14"/>
     </row>
     <row r="15" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="271" t="s">
+      <c r="A15" s="260" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="271"/>
-      <c r="C15" s="271"/>
-      <c r="D15" s="271"/>
+      <c r="B15" s="260"/>
+      <c r="C15" s="260"/>
+      <c r="D15" s="260"/>
       <c r="E15" s="67"/>
       <c r="F15" s="68"/>
       <c r="G15" s="62"/>
@@ -4686,12 +4686,12 @@
       <c r="Y15" s="24"/>
     </row>
     <row r="16" spans="1:25" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="271"/>
-      <c r="B16" s="271"/>
-      <c r="C16" s="271"/>
-      <c r="D16" s="271"/>
-      <c r="E16" s="271"/>
-      <c r="F16" s="271"/>
+      <c r="A16" s="260"/>
+      <c r="B16" s="260"/>
+      <c r="C16" s="260"/>
+      <c r="D16" s="260"/>
+      <c r="E16" s="260"/>
+      <c r="F16" s="260"/>
       <c r="G16" s="62"/>
       <c r="H16" s="69"/>
       <c r="I16" s="64"/>
@@ -4722,8 +4722,8 @@
       <c r="F17" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="272"/>
-      <c r="H17" s="273"/>
+      <c r="G17" s="261"/>
+      <c r="H17" s="262"/>
       <c r="I17" s="70"/>
       <c r="J17" s="69"/>
       <c r="K17" s="69"/>
@@ -4734,23 +4734,23 @@
       <c r="P17" s="25"/>
     </row>
     <row r="18" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="274" t="s">
+      <c r="A18" s="263" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="276">
+      <c r="B18" s="245">
         <v>4553</v>
       </c>
-      <c r="C18" s="276">
+      <c r="C18" s="245">
         <v>4713</v>
       </c>
-      <c r="D18" s="276">
+      <c r="D18" s="245">
         <v>1</v>
       </c>
-      <c r="E18" s="276">
+      <c r="E18" s="245">
         <f>C18-B18</f>
         <v>160</v>
       </c>
-      <c r="F18" s="276"/>
+      <c r="F18" s="245"/>
       <c r="G18" s="69"/>
       <c r="H18" s="69"/>
       <c r="I18" s="69"/>
@@ -4763,12 +4763,12 @@
       <c r="P18" s="25"/>
     </row>
     <row r="19" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="275"/>
-      <c r="B19" s="276"/>
-      <c r="C19" s="276"/>
-      <c r="D19" s="276"/>
-      <c r="E19" s="276"/>
-      <c r="F19" s="276"/>
+      <c r="A19" s="264"/>
+      <c r="B19" s="245"/>
+      <c r="C19" s="245"/>
+      <c r="D19" s="245"/>
+      <c r="E19" s="245"/>
+      <c r="F19" s="245"/>
       <c r="G19" s="69"/>
       <c r="H19" s="69"/>
       <c r="I19" s="69"/>
@@ -4780,12 +4780,12 @@
       <c r="V19" s="27"/>
     </row>
     <row r="20" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="275"/>
-      <c r="B20" s="276"/>
-      <c r="C20" s="276"/>
-      <c r="D20" s="276"/>
-      <c r="E20" s="276"/>
-      <c r="F20" s="276"/>
+      <c r="A20" s="264"/>
+      <c r="B20" s="245"/>
+      <c r="C20" s="245"/>
+      <c r="D20" s="245"/>
+      <c r="E20" s="245"/>
+      <c r="F20" s="245"/>
       <c r="G20" s="69"/>
       <c r="H20" s="69"/>
       <c r="I20" s="69"/>
@@ -4796,12 +4796,12 @@
       <c r="N20" s="26"/>
     </row>
     <row r="21" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="275"/>
-      <c r="B21" s="276"/>
-      <c r="C21" s="276"/>
-      <c r="D21" s="276"/>
-      <c r="E21" s="276"/>
-      <c r="F21" s="276"/>
+      <c r="A21" s="264"/>
+      <c r="B21" s="245"/>
+      <c r="C21" s="245"/>
+      <c r="D21" s="245"/>
+      <c r="E21" s="245"/>
+      <c r="F21" s="245"/>
       <c r="G21" s="69"/>
       <c r="H21" s="69"/>
       <c r="I21" s="69"/>
@@ -4812,12 +4812,12 @@
       <c r="N21" s="26"/>
     </row>
     <row r="22" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="275"/>
-      <c r="B22" s="276"/>
-      <c r="C22" s="276"/>
-      <c r="D22" s="276"/>
-      <c r="E22" s="276"/>
-      <c r="F22" s="276"/>
+      <c r="A22" s="264"/>
+      <c r="B22" s="245"/>
+      <c r="C22" s="245"/>
+      <c r="D22" s="245"/>
+      <c r="E22" s="245"/>
+      <c r="F22" s="245"/>
       <c r="G22" s="69"/>
       <c r="H22" s="69"/>
       <c r="I22" s="69"/>
@@ -4828,184 +4828,184 @@
       <c r="N22" s="26"/>
     </row>
     <row r="23" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="267" t="s">
+      <c r="A23" s="252" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="267"/>
-      <c r="C23" s="267"/>
-      <c r="D23" s="268" t="s">
+      <c r="B23" s="252"/>
+      <c r="C23" s="252"/>
+      <c r="D23" s="253" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="268"/>
-      <c r="F23" s="268"/>
-      <c r="G23" s="269" t="s">
+      <c r="E23" s="253"/>
+      <c r="F23" s="253"/>
+      <c r="G23" s="254" t="s">
         <v>94</v>
       </c>
-      <c r="H23" s="269"/>
-      <c r="I23" s="269"/>
-      <c r="J23" s="259"/>
-      <c r="K23" s="259"/>
+      <c r="H23" s="254"/>
+      <c r="I23" s="254"/>
+      <c r="J23" s="255"/>
+      <c r="K23" s="255"/>
       <c r="L23" s="24"/>
       <c r="M23" s="24"/>
       <c r="N23" s="26"/>
     </row>
     <row r="24" spans="1:28" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="247" t="s">
+      <c r="A24" s="256" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="247"/>
+      <c r="B24" s="256"/>
       <c r="C24" s="31">
         <f>E18</f>
         <v>160</v>
       </c>
-      <c r="D24" s="243" t="s">
+      <c r="D24" s="257" t="s">
         <v>95</v>
       </c>
-      <c r="E24" s="243"/>
+      <c r="E24" s="257"/>
       <c r="F24" s="31">
         <v>0</v>
       </c>
-      <c r="G24" s="247" t="s">
+      <c r="G24" s="256" t="s">
         <v>37</v>
       </c>
-      <c r="H24" s="247"/>
-      <c r="I24" s="247"/>
-      <c r="J24" s="256">
+      <c r="H24" s="256"/>
+      <c r="I24" s="256"/>
+      <c r="J24" s="258">
         <f>F37+C31</f>
         <v>5634.8</v>
       </c>
-      <c r="K24" s="256"/>
+      <c r="K24" s="258"/>
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
       <c r="N24" s="26"/>
     </row>
     <row r="25" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="246" t="s">
+      <c r="A25" s="243" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="246"/>
+      <c r="B25" s="243"/>
       <c r="C25" s="31">
         <f>IF(C24&lt;=100,(C24*C37),IF(C24&lt;=200,(C24*C38),IF(C24&lt;=300,(C24*C39),IF(C24&lt;=400,(C24*C40),IF(C24&lt;=500,(C24*C41),IF(D24&lt;=600,(D24*C42),IF(D24&lt;=700,(D24*C43),IF(D24&gt;700,(D24*C44)))))))))</f>
         <v>3672</v>
       </c>
-      <c r="D25" s="243" t="s">
+      <c r="D25" s="257" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="243"/>
+      <c r="E25" s="257"/>
       <c r="F25" s="31">
         <v>35</v>
       </c>
-      <c r="G25" s="254" t="s">
+      <c r="G25" s="265" t="s">
         <v>96</v>
       </c>
-      <c r="H25" s="254"/>
-      <c r="I25" s="254"/>
-      <c r="J25" s="256">
+      <c r="H25" s="265"/>
+      <c r="I25" s="265"/>
+      <c r="J25" s="258">
         <v>250</v>
       </c>
-      <c r="K25" s="256"/>
+      <c r="K25" s="258"/>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
       <c r="N25" s="26"/>
     </row>
     <row r="26" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="260" t="s">
+      <c r="A26" s="266" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="261"/>
-      <c r="C26" s="264">
+      <c r="B26" s="267"/>
+      <c r="C26" s="270">
         <v>825</v>
       </c>
-      <c r="D26" s="243" t="s">
+      <c r="D26" s="257" t="s">
         <v>97</v>
       </c>
-      <c r="E26" s="243"/>
+      <c r="E26" s="257"/>
       <c r="F26" s="31">
         <v>25</v>
       </c>
-      <c r="G26" s="258" t="s">
+      <c r="G26" s="272" t="s">
         <v>98</v>
       </c>
-      <c r="H26" s="258"/>
-      <c r="I26" s="258"/>
-      <c r="J26" s="266"/>
-      <c r="K26" s="266"/>
+      <c r="H26" s="272"/>
+      <c r="I26" s="272"/>
+      <c r="J26" s="273"/>
+      <c r="K26" s="273"/>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
       <c r="N26" s="26"/>
     </row>
     <row r="27" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="262"/>
-      <c r="B27" s="263"/>
-      <c r="C27" s="265"/>
-      <c r="D27" s="243" t="s">
+      <c r="A27" s="268"/>
+      <c r="B27" s="269"/>
+      <c r="C27" s="271"/>
+      <c r="D27" s="257" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="243"/>
+      <c r="E27" s="257"/>
       <c r="F27" s="31"/>
-      <c r="G27" s="254" t="s">
+      <c r="G27" s="265" t="s">
         <v>99</v>
       </c>
-      <c r="H27" s="254"/>
-      <c r="I27" s="254"/>
-      <c r="J27" s="256">
+      <c r="H27" s="265"/>
+      <c r="I27" s="265"/>
+      <c r="J27" s="258">
         <f>(J24+J25)/2</f>
         <v>2942.4</v>
       </c>
-      <c r="K27" s="256"/>
+      <c r="K27" s="258"/>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
       <c r="N27" s="26"/>
     </row>
     <row r="28" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="246" t="s">
+      <c r="A28" s="243" t="s">
         <v>100</v>
       </c>
-      <c r="B28" s="246"/>
+      <c r="B28" s="243"/>
       <c r="C28" s="31">
         <v>395</v>
       </c>
-      <c r="D28" s="243" t="s">
+      <c r="D28" s="257" t="s">
         <v>46</v>
       </c>
-      <c r="E28" s="243"/>
+      <c r="E28" s="257"/>
       <c r="F28" s="31"/>
-      <c r="G28" s="254" t="s">
+      <c r="G28" s="265" t="s">
         <v>101</v>
       </c>
-      <c r="H28" s="254"/>
-      <c r="I28" s="254"/>
-      <c r="J28" s="256">
+      <c r="H28" s="265"/>
+      <c r="I28" s="265"/>
+      <c r="J28" s="258">
         <v>0</v>
       </c>
-      <c r="K28" s="256"/>
+      <c r="K28" s="258"/>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
       <c r="N28" s="26"/>
     </row>
     <row r="29" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="246" t="s">
+      <c r="A29" s="243" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="246"/>
+      <c r="B29" s="243"/>
       <c r="C29" s="31">
         <v>166</v>
       </c>
-      <c r="D29" s="243" t="s">
+      <c r="D29" s="257" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="243"/>
+      <c r="E29" s="257"/>
       <c r="F29" s="31"/>
-      <c r="G29" s="258" t="s">
+      <c r="G29" s="272" t="s">
         <v>49</v>
       </c>
-      <c r="H29" s="258"/>
-      <c r="I29" s="258"/>
-      <c r="J29" s="259">
+      <c r="H29" s="272"/>
+      <c r="I29" s="272"/>
+      <c r="J29" s="255">
         <f>J27</f>
         <v>2942.4</v>
       </c>
-      <c r="K29" s="259"/>
+      <c r="K29" s="255"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
@@ -5025,28 +5025,28 @@
       <c r="AB29" s="5"/>
     </row>
     <row r="30" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="246" t="s">
+      <c r="A30" s="243" t="s">
         <v>102</v>
       </c>
-      <c r="B30" s="246"/>
+      <c r="B30" s="243"/>
       <c r="C30" s="31">
         <v>0</v>
       </c>
-      <c r="D30" s="243" t="s">
+      <c r="D30" s="257" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="243"/>
+      <c r="E30" s="257"/>
       <c r="F30" s="31"/>
-      <c r="G30" s="254" t="s">
+      <c r="G30" s="265" t="s">
         <v>52</v>
       </c>
-      <c r="H30" s="254"/>
-      <c r="I30" s="254"/>
-      <c r="J30" s="256">
+      <c r="H30" s="265"/>
+      <c r="I30" s="265"/>
+      <c r="J30" s="258">
         <f>J29*10%</f>
         <v>294.24</v>
       </c>
-      <c r="K30" s="256"/>
+      <c r="K30" s="258"/>
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
       <c r="N30" s="5"/>
@@ -5066,29 +5066,29 @@
       <c r="AB30" s="10"/>
     </row>
     <row r="31" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="254" t="s">
+      <c r="A31" s="265" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="254"/>
+      <c r="B31" s="265"/>
       <c r="C31" s="31">
         <f>C25+C26+C28+C29+C30</f>
         <v>5058</v>
       </c>
-      <c r="D31" s="243" t="s">
+      <c r="D31" s="257" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="243"/>
+      <c r="E31" s="257"/>
       <c r="F31" s="31"/>
-      <c r="G31" s="255" t="s">
+      <c r="G31" s="274" t="s">
         <v>55</v>
       </c>
-      <c r="H31" s="255"/>
-      <c r="I31" s="255"/>
-      <c r="J31" s="256">
+      <c r="H31" s="274"/>
+      <c r="I31" s="274"/>
+      <c r="J31" s="258">
         <f>J29+J30</f>
         <v>3236.6400000000003</v>
       </c>
-      <c r="K31" s="256"/>
+      <c r="K31" s="258"/>
       <c r="L31" s="5"/>
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
@@ -5108,23 +5108,23 @@
       <c r="AB31" s="10"/>
     </row>
     <row r="32" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="246" t="s">
+      <c r="A32" s="243" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="246"/>
+      <c r="B32" s="243"/>
       <c r="C32" s="31"/>
-      <c r="D32" s="243" t="s">
+      <c r="D32" s="257" t="s">
         <v>57</v>
       </c>
-      <c r="E32" s="243"/>
+      <c r="E32" s="257"/>
       <c r="F32" s="31"/>
-      <c r="G32" s="257" t="s">
+      <c r="G32" s="239" t="s">
         <v>45</v>
       </c>
-      <c r="H32" s="257"/>
-      <c r="I32" s="257"/>
-      <c r="J32" s="257"/>
-      <c r="K32" s="257"/>
+      <c r="H32" s="239"/>
+      <c r="I32" s="239"/>
+      <c r="J32" s="239"/>
+      <c r="K32" s="239"/>
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
       <c r="N32" s="5"/>
@@ -5144,27 +5144,27 @@
       <c r="AB32" s="10"/>
     </row>
     <row r="33" spans="1:28" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="246" t="s">
+      <c r="A33" s="243" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="246"/>
+      <c r="B33" s="243"/>
       <c r="C33" s="31"/>
-      <c r="D33" s="243" t="s">
+      <c r="D33" s="257" t="s">
         <v>59</v>
       </c>
-      <c r="E33" s="243"/>
+      <c r="E33" s="257"/>
       <c r="F33" s="31"/>
-      <c r="G33" s="248" t="s">
+      <c r="G33" s="275" t="s">
         <v>60</v>
       </c>
-      <c r="H33" s="249" t="s">
+      <c r="H33" s="242" t="s">
         <v>103</v>
       </c>
-      <c r="I33" s="249"/>
-      <c r="J33" s="250" t="s">
+      <c r="I33" s="242"/>
+      <c r="J33" s="276" t="s">
         <v>64</v>
       </c>
-      <c r="K33" s="250"/>
+      <c r="K33" s="276"/>
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
@@ -5184,30 +5184,30 @@
       <c r="AB33" s="10"/>
     </row>
     <row r="34" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="246" t="s">
+      <c r="A34" s="243" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="246"/>
+      <c r="B34" s="243"/>
       <c r="C34" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="D34" s="243" t="s">
+      <c r="D34" s="257" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="243"/>
+      <c r="E34" s="257"/>
       <c r="F34" s="31">
         <f>C24*3.23</f>
         <v>516.79999999999995</v>
       </c>
-      <c r="G34" s="248"/>
-      <c r="H34" s="251" t="s">
+      <c r="G34" s="275"/>
+      <c r="H34" s="277" t="s">
         <v>85</v>
       </c>
-      <c r="I34" s="252"/>
-      <c r="J34" s="253">
+      <c r="I34" s="278"/>
+      <c r="J34" s="279">
         <v>2.5627</v>
       </c>
-      <c r="K34" s="253"/>
+      <c r="K34" s="279"/>
       <c r="L34" s="71"/>
       <c r="M34" s="71"/>
       <c r="N34" s="5"/>
@@ -5236,16 +5236,16 @@
       <c r="C35" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="243" t="s">
+      <c r="D35" s="257" t="s">
         <v>65</v>
       </c>
-      <c r="E35" s="243"/>
+      <c r="E35" s="257"/>
       <c r="F35" s="31"/>
-      <c r="G35" s="244"/>
-      <c r="H35" s="244"/>
-      <c r="I35" s="244"/>
-      <c r="J35" s="244"/>
-      <c r="K35" s="244"/>
+      <c r="G35" s="246"/>
+      <c r="H35" s="246"/>
+      <c r="I35" s="246"/>
+      <c r="J35" s="246"/>
+      <c r="K35" s="246"/>
       <c r="L35" s="73"/>
       <c r="M35" s="73"/>
       <c r="N35" s="5"/>
@@ -5310,21 +5310,21 @@
       <c r="C37" s="76">
         <v>16.48</v>
       </c>
-      <c r="D37" s="243" t="s">
+      <c r="D37" s="257" t="s">
         <v>47</v>
       </c>
-      <c r="E37" s="243"/>
+      <c r="E37" s="257"/>
       <c r="F37" s="31">
         <f>SUM(F24:F35)</f>
         <v>576.79999999999995</v>
       </c>
-      <c r="G37" s="245" t="s">
+      <c r="G37" s="285" t="s">
         <v>66</v>
       </c>
-      <c r="H37" s="245"/>
-      <c r="I37" s="245"/>
-      <c r="J37" s="245"/>
-      <c r="K37" s="245"/>
+      <c r="H37" s="285"/>
+      <c r="I37" s="285"/>
+      <c r="J37" s="285"/>
+      <c r="K37" s="285"/>
       <c r="L37" s="71"/>
       <c r="M37" s="71"/>
       <c r="N37" s="5"/>
@@ -5353,16 +5353,16 @@
       <c r="C38" s="76">
         <v>22.95</v>
       </c>
-      <c r="D38" s="244"/>
-      <c r="E38" s="244"/>
-      <c r="F38" s="244"/>
-      <c r="G38" s="246" t="s">
+      <c r="D38" s="246"/>
+      <c r="E38" s="246"/>
+      <c r="F38" s="246"/>
+      <c r="G38" s="243" t="s">
         <v>104</v>
       </c>
-      <c r="H38" s="246"/>
-      <c r="I38" s="246"/>
-      <c r="J38" s="246"/>
-      <c r="K38" s="246"/>
+      <c r="H38" s="243"/>
+      <c r="I38" s="243"/>
+      <c r="J38" s="243"/>
+      <c r="K38" s="243"/>
       <c r="L38" s="79"/>
       <c r="M38" s="79"/>
       <c r="N38" s="35"/>
@@ -5391,16 +5391,16 @@
       <c r="C39" s="76">
         <v>34.26</v>
       </c>
-      <c r="D39" s="244"/>
-      <c r="E39" s="244"/>
-      <c r="F39" s="244"/>
-      <c r="G39" s="247" t="s">
+      <c r="D39" s="246"/>
+      <c r="E39" s="246"/>
+      <c r="F39" s="246"/>
+      <c r="G39" s="256" t="s">
         <v>105</v>
       </c>
-      <c r="H39" s="247"/>
-      <c r="I39" s="247"/>
-      <c r="J39" s="247"/>
-      <c r="K39" s="247"/>
+      <c r="H39" s="256"/>
+      <c r="I39" s="256"/>
+      <c r="J39" s="256"/>
+      <c r="K39" s="256"/>
       <c r="L39" s="79"/>
       <c r="M39" s="79"/>
       <c r="N39" s="37"/>
@@ -5429,16 +5429,16 @@
       <c r="C40" s="76">
         <v>39.15</v>
       </c>
-      <c r="D40" s="244"/>
-      <c r="E40" s="244"/>
-      <c r="F40" s="244"/>
-      <c r="G40" s="245" t="s">
+      <c r="D40" s="246"/>
+      <c r="E40" s="246"/>
+      <c r="F40" s="246"/>
+      <c r="G40" s="285" t="s">
         <v>106</v>
       </c>
-      <c r="H40" s="245"/>
-      <c r="I40" s="245"/>
-      <c r="J40" s="245"/>
-      <c r="K40" s="245"/>
+      <c r="H40" s="285"/>
+      <c r="I40" s="285"/>
+      <c r="J40" s="285"/>
+      <c r="K40" s="285"/>
       <c r="L40" s="79"/>
       <c r="M40" s="79"/>
       <c r="N40" s="5"/>
@@ -5467,16 +5467,16 @@
       <c r="C41" s="76">
         <v>41.36</v>
       </c>
-      <c r="D41" s="244"/>
-      <c r="E41" s="244"/>
-      <c r="F41" s="244"/>
-      <c r="G41" s="246" t="s">
+      <c r="D41" s="246"/>
+      <c r="E41" s="246"/>
+      <c r="F41" s="246"/>
+      <c r="G41" s="243" t="s">
         <v>107</v>
       </c>
-      <c r="H41" s="246"/>
-      <c r="I41" s="246"/>
-      <c r="J41" s="246"/>
-      <c r="K41" s="246"/>
+      <c r="H41" s="243"/>
+      <c r="I41" s="243"/>
+      <c r="J41" s="243"/>
+      <c r="K41" s="243"/>
       <c r="L41" s="5"/>
       <c r="M41" s="5"/>
     </row>
@@ -5490,16 +5490,16 @@
       <c r="C42" s="76">
         <v>42.78</v>
       </c>
-      <c r="D42" s="238" t="s">
+      <c r="D42" s="280" t="s">
         <v>108</v>
       </c>
-      <c r="E42" s="238"/>
-      <c r="F42" s="238"/>
-      <c r="G42" s="238"/>
-      <c r="H42" s="238"/>
-      <c r="I42" s="238"/>
-      <c r="J42" s="238"/>
-      <c r="K42" s="238"/>
+      <c r="E42" s="280"/>
+      <c r="F42" s="280"/>
+      <c r="G42" s="280"/>
+      <c r="H42" s="280"/>
+      <c r="I42" s="280"/>
+      <c r="J42" s="280"/>
+      <c r="K42" s="280"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -5528,16 +5528,16 @@
       <c r="C43" s="76">
         <v>43.92</v>
       </c>
-      <c r="D43" s="239" t="s">
+      <c r="D43" s="281" t="s">
         <v>109</v>
       </c>
-      <c r="E43" s="239"/>
-      <c r="F43" s="239"/>
-      <c r="G43" s="239"/>
-      <c r="H43" s="239"/>
-      <c r="I43" s="239"/>
-      <c r="J43" s="239"/>
-      <c r="K43" s="239"/>
+      <c r="E43" s="281"/>
+      <c r="F43" s="281"/>
+      <c r="G43" s="281"/>
+      <c r="H43" s="281"/>
+      <c r="I43" s="281"/>
+      <c r="J43" s="281"/>
+      <c r="K43" s="281"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -5566,14 +5566,14 @@
       <c r="C44" s="82">
         <v>48.84</v>
       </c>
-      <c r="D44" s="240"/>
-      <c r="E44" s="240"/>
-      <c r="F44" s="240"/>
-      <c r="G44" s="240"/>
-      <c r="H44" s="240"/>
-      <c r="I44" s="240"/>
-      <c r="J44" s="240"/>
-      <c r="K44" s="240"/>
+      <c r="D44" s="282"/>
+      <c r="E44" s="282"/>
+      <c r="F44" s="282"/>
+      <c r="G44" s="282"/>
+      <c r="H44" s="282"/>
+      <c r="I44" s="282"/>
+      <c r="J44" s="282"/>
+      <c r="K44" s="282"/>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -5593,19 +5593,19 @@
       <c r="AB44" s="2"/>
     </row>
     <row r="45" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="241" t="s">
+      <c r="A45" s="283" t="s">
         <v>110</v>
       </c>
-      <c r="B45" s="241"/>
-      <c r="C45" s="241"/>
-      <c r="D45" s="241"/>
-      <c r="E45" s="241"/>
-      <c r="F45" s="241"/>
-      <c r="G45" s="241"/>
-      <c r="H45" s="241"/>
-      <c r="I45" s="241"/>
-      <c r="J45" s="241"/>
-      <c r="K45" s="241"/>
+      <c r="B45" s="283"/>
+      <c r="C45" s="283"/>
+      <c r="D45" s="283"/>
+      <c r="E45" s="283"/>
+      <c r="F45" s="283"/>
+      <c r="G45" s="283"/>
+      <c r="H45" s="283"/>
+      <c r="I45" s="283"/>
+      <c r="J45" s="283"/>
+      <c r="K45" s="283"/>
       <c r="L45" s="39"/>
       <c r="M45" s="39"/>
       <c r="N45" s="39"/>
@@ -5625,17 +5625,17 @@
       <c r="AB45" s="39"/>
     </row>
     <row r="46" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="241"/>
-      <c r="B46" s="241"/>
-      <c r="C46" s="241"/>
-      <c r="D46" s="241"/>
-      <c r="E46" s="241"/>
-      <c r="F46" s="241"/>
-      <c r="G46" s="241"/>
-      <c r="H46" s="241"/>
-      <c r="I46" s="241"/>
-      <c r="J46" s="241"/>
-      <c r="K46" s="241"/>
+      <c r="A46" s="283"/>
+      <c r="B46" s="283"/>
+      <c r="C46" s="283"/>
+      <c r="D46" s="283"/>
+      <c r="E46" s="283"/>
+      <c r="F46" s="283"/>
+      <c r="G46" s="283"/>
+      <c r="H46" s="283"/>
+      <c r="I46" s="283"/>
+      <c r="J46" s="283"/>
+      <c r="K46" s="283"/>
       <c r="L46" s="6"/>
       <c r="M46" s="6"/>
       <c r="N46" s="6"/>
@@ -5691,11 +5691,11 @@
       <c r="C49" s="6"/>
     </row>
     <row r="50" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I50" s="242" t="s">
+      <c r="I50" s="284" t="s">
         <v>111</v>
       </c>
-      <c r="J50" s="242"/>
-      <c r="K50" s="242"/>
+      <c r="J50" s="284"/>
+      <c r="K50" s="284"/>
     </row>
     <row r="51" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="52" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5704,36 +5704,59 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="101">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A1:B4"/>
-    <mergeCell ref="C1:K2"/>
-    <mergeCell ref="C3:K3"/>
-    <mergeCell ref="C4:K4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="D42:K42"/>
+    <mergeCell ref="D43:K44"/>
+    <mergeCell ref="A45:K46"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="G37:K37"/>
+    <mergeCell ref="D38:F41"/>
+    <mergeCell ref="G38:K38"/>
+    <mergeCell ref="G39:K39"/>
+    <mergeCell ref="G40:K40"/>
+    <mergeCell ref="G41:K41"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="G32:K32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="A26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="D27:E27"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="G23:I23"/>
@@ -5752,59 +5775,36 @@
     <mergeCell ref="D18:D22"/>
     <mergeCell ref="E18:E22"/>
     <mergeCell ref="F18:F22"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="A26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="G32:K32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="D42:K42"/>
-    <mergeCell ref="D43:K44"/>
-    <mergeCell ref="A45:K46"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="G35:K35"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="G37:K37"/>
-    <mergeCell ref="D38:F41"/>
-    <mergeCell ref="G38:K38"/>
-    <mergeCell ref="G39:K39"/>
-    <mergeCell ref="G40:K40"/>
-    <mergeCell ref="G41:K41"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="A1:B4"/>
+    <mergeCell ref="C1:K2"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="C4:K4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0.35433070866141736" footer="0.31496062992125984"/>

</xml_diff>